<commit_message>
ignore temp excel files
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
@@ -1,25 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A63272-B250-3C46-BFE4-9426E84515E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28340" tabRatio="500" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="notify_lookup" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="termby_lookup" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="notified_lookup" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="proof_lookup" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="letter_sent_death_lookup" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="client_death_notifications" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="date_of_death_lookup" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="deputy_death_notifications" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="deputy_date_of_death_lookup" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="notify_lookup" sheetId="1" r:id="rId1"/>
+    <sheet name="termby_lookup" sheetId="2" r:id="rId2"/>
+    <sheet name="notified_lookup" sheetId="3" r:id="rId3"/>
+    <sheet name="proof_lookup" sheetId="4" r:id="rId4"/>
+    <sheet name="letter_sent_death_lookup" sheetId="5" r:id="rId5"/>
+    <sheet name="client_death_notifications" sheetId="6" r:id="rId6"/>
+    <sheet name="date_of_death_lookup" sheetId="7" r:id="rId7"/>
+    <sheet name="deputy_death_notifications" sheetId="8" r:id="rId8"/>
+    <sheet name="deputy_date_of_death_lookup" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -28,265 +42,240 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="64">
-  <si>
-    <t xml:space="preserve">casrec_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Casrec Desc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sirius_mapping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Death of client</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notify</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Term by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proof</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Letter Sent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">table_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">column_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_pk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fk_children</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fk_parents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">casrec_table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">annex_column_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">casrec_column_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">requires_transformation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lookup_table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">additional_columns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_complete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">death_notifications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">death_notification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not mapped</t>
-  </si>
-  <si>
-    <t xml:space="preserve">person_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">persons:id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proofofdeathreceived</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datelettersentout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conditional_lookup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">letter_sent_death_lookup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Term Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datedeathcertificatereceived</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proof_lookup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datenotified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notified_lookup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notifiedby</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str</t>
-  </si>
-  <si>
-    <t xml:space="preserve">termby_lookup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notifiedbyother</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notificationmethod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notify_lookup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Migrated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Term Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deputy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deputy_date_of_death_lookup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OTHER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Migration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DECEASED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disch Death</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="63">
+  <si>
+    <t>casrec_code</t>
+  </si>
+  <si>
+    <t>entity</t>
+  </si>
+  <si>
+    <t>Casrec Desc</t>
+  </si>
+  <si>
+    <t>sirius_mapping</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Death of client</t>
+  </si>
+  <si>
+    <t>Notify</t>
+  </si>
+  <si>
+    <t>Term by</t>
+  </si>
+  <si>
+    <t>Notified</t>
+  </si>
+  <si>
+    <t>Proof</t>
+  </si>
+  <si>
+    <t>Letter Sent</t>
+  </si>
+  <si>
+    <t>table_name</t>
+  </si>
+  <si>
+    <t>column_name</t>
+  </si>
+  <si>
+    <t>data_type</t>
+  </si>
+  <si>
+    <t>is_pk</t>
+  </si>
+  <si>
+    <t>fk_children</t>
+  </si>
+  <si>
+    <t>fk_parents</t>
+  </si>
+  <si>
+    <t>casrec_table</t>
+  </si>
+  <si>
+    <t>annex_column_name</t>
+  </si>
+  <si>
+    <t>casrec_column_name</t>
+  </si>
+  <si>
+    <t>requires_transformation</t>
+  </si>
+  <si>
+    <t>lookup_table</t>
+  </si>
+  <si>
+    <t>default_value</t>
+  </si>
+  <si>
+    <t>calculated</t>
+  </si>
+  <si>
+    <t>additional_columns</t>
+  </si>
+  <si>
+    <t>is_complete</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>death_notifications</t>
+  </si>
+  <si>
+    <t>death_notification</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>not mapped</t>
+  </si>
+  <si>
+    <t>person_id</t>
+  </si>
+  <si>
+    <t>persons:id</t>
+  </si>
+  <si>
+    <t>proofofdeathreceived</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>datelettersentout</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>PAT</t>
+  </si>
+  <si>
+    <t>conditional_lookup</t>
+  </si>
+  <si>
+    <t>letter_sent_death_lookup</t>
+  </si>
+  <si>
+    <t>Term Type</t>
+  </si>
+  <si>
+    <t>datedeathcertificatereceived</t>
+  </si>
+  <si>
+    <t>datenotified</t>
+  </si>
+  <si>
+    <t>notified_lookup</t>
+  </si>
+  <si>
+    <t>notifiedby</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>termby_lookup</t>
+  </si>
+  <si>
+    <t>notifiedbyother</t>
+  </si>
+  <si>
+    <t>notificationmethod</t>
+  </si>
+  <si>
+    <t>notify_lookup</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Migrated</t>
+  </si>
+  <si>
+    <t>Term Date</t>
+  </si>
+  <si>
+    <t>Deputy</t>
+  </si>
+  <si>
+    <t>deputy_date_of_death_lookup</t>
+  </si>
+  <si>
+    <t>Stat</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
+    <t>Migration</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>DECEASED</t>
+  </si>
+  <si>
+    <t>Disch Death</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="D\-MMM\-YY"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="&quot;Google Sans&quot;"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -311,123 +300,77 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -486,28 +429,336 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF222222"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:24" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,7 +792,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -573,7 +824,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -599,7 +850,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -625,7 +876,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -651,7 +902,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -677,7 +928,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:24" ht="15">
       <c r="E7" s="7"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -699,7 +950,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -721,7 +972,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:24" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -747,35 +998,27 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:24" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -809,7 +1052,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -841,7 +1084,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -867,7 +1110,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -893,7 +1136,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -919,7 +1162,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:24" ht="15">
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -941,7 +1184,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -967,7 +1210,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -989,7 +1232,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:24" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1015,35 +1258,27 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:24" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1077,7 +1312,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1109,7 +1344,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -1135,7 +1370,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -1161,7 +1396,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:24" ht="15">
       <c r="E5" s="7"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1183,7 +1418,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1209,7 +1444,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -1235,7 +1470,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1257,7 +1492,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:24" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1283,35 +1518,27 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:24" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1345,7 +1572,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1377,7 +1604,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -1403,7 +1630,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:24" ht="15">
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1425,7 +1652,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -1451,7 +1678,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1477,7 +1704,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -1503,7 +1730,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1525,7 +1752,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:24" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1551,35 +1778,27 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:24" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1613,7 +1832,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1645,7 +1864,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:24" ht="15">
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1667,7 +1886,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -1693,7 +1912,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -1719,7 +1938,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1745,7 +1964,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -1771,7 +1990,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1793,7 +2012,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:24" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1819,54 +2038,45 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="14.43"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="19.5" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="22.5" customWidth="1"/>
+    <col min="12" max="12" width="20.5" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" customWidth="1"/>
+    <col min="18" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:17" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1919,7 +2129,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:17" ht="15">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1932,15 +2142,15 @@
       <c r="D2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="E2" s="4" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:17" ht="15">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1953,8 +2163,8 @@
       <c r="D3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="4" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="E3" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1964,7 +2174,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:17" ht="15">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1977,16 +2187,16 @@
       <c r="D4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="4" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="E4" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="12"/>
-      <c r="M4" s="5" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="M4" s="5" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="N4" s="5"/>
@@ -1995,7 +2205,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:17" ht="15">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -2008,8 +2218,8 @@
       <c r="D5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="4" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="E5" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -2033,7 +2243,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:17" ht="15">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -2046,32 +2256,20 @@
       <c r="D6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="4" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="E6" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>44</v>
-      </c>
+      <c r="H6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="12"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
-      <c r="O6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O6" s="5"/>
+      <c r="P6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" ht="15">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -2079,13 +2277,13 @@
         <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="4" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="E7" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H7" s="5" t="s">
@@ -2098,7 +2296,7 @@
         <v>40</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
@@ -2109,7 +2307,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:17" ht="15">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -2117,13 +2315,13 @@
         <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="4" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="E8" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H8" s="5" t="s">
@@ -2136,7 +2334,7 @@
         <v>40</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
@@ -2147,7 +2345,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:17" ht="15">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -2155,13 +2353,13 @@
         <v>28</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="4" t="n">
-        <f aca="false">FALSE()</f>
+        <v>47</v>
+      </c>
+      <c r="E9" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H9" s="5"/>
@@ -2175,7 +2373,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:17" ht="15">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -2183,13 +2381,13 @@
         <v>28</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="4" t="n">
-        <f aca="false">FALSE()</f>
+        <v>47</v>
+      </c>
+      <c r="E10" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H10" s="5" t="s">
@@ -2202,7 +2400,7 @@
         <v>40</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
@@ -2213,7 +2411,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:17" ht="15">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -2221,13 +2419,13 @@
         <v>28</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="4" t="n">
-        <f aca="false">FALSE()</f>
+        <v>47</v>
+      </c>
+      <c r="E11" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -2237,7 +2435,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="12"/>
       <c r="M11" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -2245,35 +2443,27 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:24" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2307,7 +2497,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2316,7 +2506,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2339,7 +2529,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2365,7 +2555,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -2391,7 +2581,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2417,7 +2607,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2443,7 +2633,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2469,7 +2659,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2491,7 +2681,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:24" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2517,54 +2707,46 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="14.43"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="22.5" customWidth="1"/>
+    <col min="12" max="12" width="20.5" customWidth="1"/>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="14" max="14" width="20.5" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" customWidth="1"/>
+    <col min="18" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:17" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -2617,7 +2799,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:17" ht="15">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -2630,15 +2812,15 @@
       <c r="D2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="E2" s="4" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:17" ht="15">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -2651,8 +2833,8 @@
       <c r="D3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="4" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="E3" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -2662,7 +2844,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:17" ht="15">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -2675,16 +2857,16 @@
       <c r="D4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="4" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="E4" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="12"/>
-      <c r="M4" s="5" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="M4" s="5" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="N4" s="5"/>
@@ -2693,7 +2875,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:17" ht="15">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -2706,32 +2888,32 @@
       <c r="D5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="4" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="E5" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>40</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:17" ht="15">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -2744,32 +2926,32 @@
       <c r="D6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="4" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="E6" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>9</v>
+        <v>55</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>40</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:17" ht="15">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -2777,37 +2959,37 @@
         <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="4" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="E7" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>8</v>
+        <v>55</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>40</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:17" ht="15">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -2815,13 +2997,13 @@
         <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="4" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="E8" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H8" s="5"/>
@@ -2829,17 +3011,17 @@
       <c r="K8" s="5"/>
       <c r="L8" s="14"/>
       <c r="M8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:17" ht="15">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -2847,13 +3029,13 @@
         <v>28</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="4" t="n">
-        <f aca="false">FALSE()</f>
+        <v>47</v>
+      </c>
+      <c r="E9" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H9" s="5"/>
@@ -2861,7 +3043,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="12"/>
       <c r="M9" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -2869,7 +3051,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:17" ht="15">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -2877,13 +3059,13 @@
         <v>28</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="4" t="n">
-        <f aca="false">FALSE()</f>
+        <v>47</v>
+      </c>
+      <c r="E10" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H10" s="5"/>
@@ -2891,7 +3073,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="14"/>
       <c r="M10" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5" t="s">
@@ -2901,7 +3083,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:17" ht="15">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -2909,13 +3091,13 @@
         <v>28</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="4" t="n">
-        <f aca="false">FALSE()</f>
+        <v>47</v>
+      </c>
+      <c r="E11" s="4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H11" s="5"/>
@@ -2923,7 +3105,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="12"/>
       <c r="M11" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -2931,35 +3113,25 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:24" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2993,16 +3165,16 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+    <row r="2" spans="1:24" ht="15">
+      <c r="A2" s="2">
         <v>99</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3025,7 +3197,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -3050,7 +3222,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -3076,7 +3248,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -3102,7 +3274,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -3128,7 +3300,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3154,7 +3326,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3176,7 +3348,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:24" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3202,14 +3374,9 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
death fix - forgot to add after merging the whole table condition change
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFEFAC3-E17B-9848-8ED2-FEF6D4BF194C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07E2FD5-2BB1-E64E-BC2B-C3C010F46B10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28340" tabRatio="500" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="28340" tabRatio="500" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notify_type_lookup" sheetId="11" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="70">
   <si>
     <t>casrec_code</t>
   </si>
@@ -169,24 +169,12 @@
     <t>PAT</t>
   </si>
   <si>
-    <t>conditional_lookup</t>
-  </si>
-  <si>
-    <t>letter_sent_death_lookup</t>
-  </si>
-  <si>
-    <t>Term Type</t>
-  </si>
-  <si>
     <t>datedeathcertificatereceived</t>
   </si>
   <si>
     <t>datenotified</t>
   </si>
   <si>
-    <t>notified_lookup</t>
-  </si>
-  <si>
     <t>notifiedby</t>
   </si>
   <si>
@@ -208,12 +196,6 @@
     <t>Deputy</t>
   </si>
   <si>
-    <t>deputy_date_of_death_lookup</t>
-  </si>
-  <si>
-    <t>Stat</t>
-  </si>
-  <si>
     <t>OTHER</t>
   </si>
   <si>
@@ -232,10 +214,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>proof_lookup
-proof_boolean_lookup</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -248,14 +226,6 @@
     <t>Death of client no</t>
   </si>
   <si>
-    <t>notify_lookup
-notify_type_lookup</t>
-  </si>
-  <si>
-    <t>termby_lookup
-termby_type_lookup</t>
-  </si>
-  <si>
     <t>Letter</t>
   </si>
   <si>
@@ -281,6 +251,12 @@
   </si>
   <si>
     <t>deputy</t>
+  </si>
+  <si>
+    <t>termby_lookup</t>
+  </si>
+  <si>
+    <t>notify_type_lookup</t>
   </si>
 </sst>
 </file>
@@ -301,26 +277,26 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -820,7 +796,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -852,7 +828,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -884,7 +860,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
@@ -916,7 +892,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="2"/>
@@ -948,7 +924,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
@@ -979,7 +955,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="2"/>
@@ -1010,7 +986,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1073,7 +1049,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
+      <selection pane="bottomLeft" activeCell="O5" sqref="O5:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -1245,22 +1221,16 @@
         <v>0</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="13" t="s">
         <v>53</v>
       </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="13"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="O5" s="5"/>
       <c r="P5" s="6" t="s">
         <v>36</v>
       </c>
@@ -1273,7 +1243,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>38</v>
@@ -1283,22 +1253,16 @@
         <v>0</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="14" t="s">
         <v>53</v>
       </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="14"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
-      <c r="O6" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="O6" s="5"/>
       <c r="P6" s="6" t="s">
         <v>36</v>
       </c>
@@ -1311,7 +1275,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>38</v>
@@ -1321,22 +1285,16 @@
         <v>0</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="14" t="s">
         <v>53</v>
       </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="14"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
-      <c r="O7" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="O7" s="5"/>
       <c r="P7" s="6" t="s">
         <v>36</v>
       </c>
@@ -1349,10 +1307,10 @@
         <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E8" s="4" t="b">
         <f>FALSE()</f>
@@ -1363,12 +1321,10 @@
       <c r="K8" s="5"/>
       <c r="L8" s="14"/>
       <c r="M8" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="N8" s="5"/>
-      <c r="O8" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="O8" s="5"/>
       <c r="P8" s="6" t="s">
         <v>36</v>
       </c>
@@ -1381,10 +1337,10 @@
         <v>28</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E9" s="4" t="b">
         <f>FALSE()</f>
@@ -1395,7 +1351,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="12"/>
       <c r="M9" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -1411,10 +1367,10 @@
         <v>28</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E10" s="4" t="b">
         <f>FALSE()</f>
@@ -1425,12 +1381,10 @@
       <c r="K10" s="5"/>
       <c r="L10" s="14"/>
       <c r="M10" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="N10" s="5"/>
-      <c r="O10" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="O10" s="5"/>
       <c r="P10" s="6" t="s">
         <v>36</v>
       </c>
@@ -1443,10 +1397,10 @@
         <v>28</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E11" s="4" t="b">
         <f>FALSE()</f>
@@ -1457,7 +1411,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="12"/>
       <c r="M11" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -1525,10 +1479,10 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1784,11 +1738,11 @@
     </row>
     <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D2" s="5" t="b">
         <v>1</v>
@@ -1816,11 +1770,11 @@
     </row>
     <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D3" s="6" t="b">
         <v>0</v>
@@ -2570,14 +2524,14 @@
     </row>
     <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2602,14 +2556,14 @@
     </row>
     <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -2634,14 +2588,14 @@
     </row>
     <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
@@ -2842,11 +2796,11 @@
     </row>
     <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
@@ -3575,7 +3529,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P4" sqref="P4"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -3698,7 +3652,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="32">
+    <row r="4" spans="1:17" ht="15">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -3721,17 +3675,11 @@
       <c r="J4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>61</v>
-      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="15"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
-      <c r="O4" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="O4" s="5"/>
       <c r="P4" s="6" t="s">
         <v>31</v>
       </c>
@@ -3759,17 +3707,11 @@
       <c r="J5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="O5" s="5"/>
       <c r="P5" s="6" t="s">
         <v>36</v>
       </c>
@@ -3782,7 +3724,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>38</v>
@@ -3799,7 +3741,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15">
@@ -3810,7 +3752,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>38</v>
@@ -3825,22 +3767,16 @@
       <c r="J7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="12"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
-      <c r="O7" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="O7" s="5"/>
       <c r="P7" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="32">
+    <row r="8" spans="1:17" ht="16">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -3848,10 +3784,10 @@
         <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E8" s="4" t="b">
         <f>FALSE()</f>
@@ -3863,17 +3799,13 @@
       <c r="J8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="K8" s="5"/>
       <c r="L8" s="15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
-      <c r="O8" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="O8" s="5"/>
       <c r="P8" s="6" t="s">
         <v>36</v>
       </c>
@@ -3886,10 +3818,10 @@
         <v>28</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E9" s="4" t="b">
         <f>FALSE()</f>
@@ -3906,7 +3838,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="32">
+    <row r="10" spans="1:17" ht="16">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -3914,10 +3846,10 @@
         <v>28</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E10" s="4" t="b">
         <f>FALSE()</f>
@@ -3929,17 +3861,13 @@
       <c r="J10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="K10" s="5"/>
       <c r="L10" s="15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="O10" s="5"/>
       <c r="P10" s="6" t="s">
         <v>36</v>
       </c>
@@ -3952,10 +3880,10 @@
         <v>28</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E11" s="4" t="b">
         <f>FALSE()</f>
@@ -3968,7 +3896,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="12"/>
       <c r="M11" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>

</xml_diff>

<commit_message>
In 746 reindex lookups (#45)
* add new `integration` container

* chAnge integration container to prepare

* updated defs

* fix a few problem mapping things
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61B0C24-B42D-6543-8D78-46711B88E9E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDBFBAF-B8FD-EB46-9C51-FF661C5811B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="28340" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="28340" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notify_type_lookup" sheetId="11" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="72">
   <si>
     <t>casrec_code</t>
   </si>
@@ -2764,7 +2764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3555,9 +3555,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -3917,9 +3917,7 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="H11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="12"/>

</xml_diff>

<commit_message>
update status and client addresses
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farzanfatemifar/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDBFBAF-B8FD-EB46-9C51-FF661C5811B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="28340" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="27420" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="notify_type_lookup" sheetId="11" r:id="rId1"/>
@@ -25,8 +24,11 @@
     <sheet name="deputy_death_notifications" sheetId="8" r:id="rId10"/>
     <sheet name="deputy_date_of_death_lookup" sheetId="9" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,9 +38,6 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="71">
   <si>
     <t>casrec_code</t>
   </si>
@@ -209,9 +208,6 @@
   </si>
   <si>
     <t>Disch Death</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
   <si>
     <t>Y</t>
@@ -268,11 +264,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -754,19 +750,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,7 +796,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>4</v>
       </c>
@@ -809,7 +805,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -832,7 +828,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>6</v>
       </c>
@@ -841,7 +837,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -864,7 +860,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -873,7 +869,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
@@ -896,7 +892,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -905,7 +901,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="2"/>
@@ -928,7 +924,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -937,7 +933,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
@@ -960,7 +956,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0</v>
       </c>
@@ -968,7 +964,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="2"/>
@@ -991,7 +987,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="15">
+    <row r="8" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -999,7 +995,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1022,7 +1018,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1048,7 +1044,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1056,7 +1052,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1065,7 +1061,7 @@
       <selection pane="bottomLeft" activeCell="O5" sqref="O5:O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -1087,7 +1083,7 @@
     <col min="18" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1140,7 +1136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1161,7 +1157,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15">
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1185,7 +1181,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1216,7 +1212,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15">
+    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1248,7 +1244,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15">
+    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1280,7 +1276,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15">
+    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -1312,7 +1308,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15">
+    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -1342,7 +1338,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15">
+    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -1372,7 +1368,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15">
+    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1402,7 +1398,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15">
+    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -1432,7 +1428,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1440,19 +1436,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1486,7 +1482,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>99</v>
       </c>
@@ -1518,7 +1514,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -1543,7 +1539,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -1569,7 +1565,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -1595,7 +1591,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1621,7 +1617,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -1647,7 +1643,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1669,7 +1665,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1695,7 +1691,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1703,19 +1699,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1749,13 +1745,13 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="5" t="b">
         <v>1</v>
@@ -1781,13 +1777,13 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="6" t="b">
         <v>0</v>
@@ -1813,7 +1809,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1835,7 +1831,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -1861,7 +1857,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1887,7 +1883,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -1913,7 +1909,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1935,7 +1931,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1961,7 +1957,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1969,19 +1965,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2015,7 +2011,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2047,7 +2043,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2073,7 +2069,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2095,7 +2091,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2121,7 +2117,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2147,7 +2143,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2173,7 +2169,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2195,7 +2191,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2221,7 +2217,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -2229,19 +2225,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2275,7 +2271,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2307,7 +2303,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2333,7 +2329,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -2359,7 +2355,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2385,7 +2381,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2411,7 +2407,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E7" s="7"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2433,7 +2429,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2455,7 +2451,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2481,7 +2477,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -2489,19 +2485,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2535,13 +2531,13 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -2567,16 +2563,16 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -2599,16 +2595,16 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
@@ -2631,7 +2627,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2657,7 +2653,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2679,7 +2675,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2705,7 +2701,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2727,7 +2723,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2753,7 +2749,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -2761,19 +2757,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2807,16 +2803,16 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2839,16 +2835,16 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -2871,12 +2867,12 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>49</v>
@@ -2902,7 +2898,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2928,7 +2924,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2950,7 +2946,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2976,7 +2972,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2998,7 +2994,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3024,7 +3020,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -3032,19 +3028,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3078,7 +3074,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3110,7 +3106,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -3136,7 +3132,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -3162,7 +3158,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E5" s="7"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -3184,7 +3180,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -3210,7 +3206,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3236,7 +3232,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3258,7 +3254,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3284,7 +3280,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -3292,19 +3288,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3338,7 +3334,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3370,7 +3366,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -3392,7 +3388,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -3418,7 +3414,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -3444,7 +3440,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -3470,7 +3466,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3496,7 +3492,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3518,7 +3514,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3544,7 +3540,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -3552,15 +3548,15 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -3582,7 +3578,7 @@
     <col min="18" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -3635,7 +3631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -3656,7 +3652,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15">
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -3680,7 +3676,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -3712,7 +3708,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15">
+    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -3744,7 +3740,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15">
+    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -3769,10 +3765,10 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -3804,7 +3800,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16">
+    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -3829,7 +3825,7 @@
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
@@ -3838,7 +3834,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15">
+    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -3866,7 +3862,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="16">
+    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -3891,7 +3887,7 @@
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
@@ -3900,7 +3896,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15">
+    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -3930,7 +3926,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>